<commit_message>
More work on the spreadsheet.
</commit_message>
<xml_diff>
--- a/data/EnergyEfficiencyData.xlsx
+++ b/data/EnergyEfficiencyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/ReboundPaper2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A35FF04-E115-0E47-9AE6-413DA46781AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E0C3F7-601D-EF48-9FC0-D492212156A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31060" yWindow="460" windowWidth="19540" windowHeight="27340" activeTab="4" xr2:uid="{D5A3B5ED-380C-904B-9F1C-82A1AD5F55AA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{D5A3B5ED-380C-904B-9F1C-82A1AD5F55AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -49,34 +48,70 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CCD4E8CF-66CA-9A43-BEB3-4ADCD767A0F4}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Marginal Propensity to Consume [-]</t>
+        </r>
       </text>
     </comment>
     <comment ref="B1" authorId="1" shapeId="0" xr:uid="{163B1487-8EB5-C74D-BB80-099EE5DECE5E}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Reserve Rate in the U.S. [-]</t>
+        </r>
       </text>
     </comment>
     <comment ref="C1" authorId="2" shapeId="0" xr:uid="{C9AAF3F9-AB53-B74F-AAB3-18867750431D}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Energy total final consumption for the US in 2016 [MJ]. Source: IEA extended energy balances 2018.</t>
+        </r>
       </text>
     </comment>
     <comment ref="D1" authorId="3" shapeId="0" xr:uid="{EDB7354F-9C95-8646-AA76-D4E19F4DD586}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     U.S. Gross Domestic Product [2016 USD]. Source: Bureau of Economic Analysis, National income and product accounts, Ta- ble 1.1.5. Gross Domestic Product (https://apps.bea.gov/iTable/iTable.cfm?reqid=19&amp;step=2)</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -93,26 +128,145 @@
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8F9C5BBE-53F8-BF46-AE84-E7DFA054348B}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Price of final energy [$/MJ]</t>
+        </r>
       </text>
     </comment>
     <comment ref="D1" authorId="1" shapeId="0" xr:uid="{19F8E058-A8E5-854A-B0B8-AF68F743BEC5}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Lifetime cost of final energy over the lifetime of the device in base case.</t>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Comment:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    Lifetime cost of final energy over the lifetime of the device in base case.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{5AD6B710-EB47-624A-8A2B-FFA78E02B50F}">
+    <comment ref="G1" authorId="2" shapeId="0" xr:uid="{5AD6B710-EB47-624A-8A2B-FFA78E02B50F}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Lifetime cost of final energy for the energy efficient case.</t>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Comment:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    Lifetime cost of final energy for the energy efficient case.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -129,26 +283,145 @@
   <commentList>
     <comment ref="B22" authorId="0" shapeId="0" xr:uid="{8A4A3D01-E799-5040-9A80-B09F68D5AC04}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Includes replacement cost</t>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Comment:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    Includes replacement cost</t>
+        </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="1" shapeId="0" xr:uid="{AD5239DB-E9DD-DA4E-B1B9-11F2751D8B5F}">
+    <comment ref="B49" authorId="1" shapeId="0" xr:uid="{AD5239DB-E9DD-DA4E-B1B9-11F2751D8B5F}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Includes replacement cost</t>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Comment:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    Includes replacement cost</t>
+        </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="2" shapeId="0" xr:uid="{CB3A4D37-2BE9-2B40-8B52-36B3DA26E41C}">
+    <comment ref="B55" authorId="2" shapeId="0" xr:uid="{CB3A4D37-2BE9-2B40-8B52-36B3DA26E41C}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ratio of embodied energy in LED vs. incandescent lights. [-]</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -156,7 +429,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
   <si>
     <t>People</t>
   </si>
@@ -269,27 +542,12 @@
     <t>$/yr</t>
   </si>
   <si>
-    <t>Ann emb enrg</t>
-  </si>
-  <si>
     <t>kW-hr/yr</t>
   </si>
   <si>
     <t>https://www.amazon.com/60-Watt-Reveal-Crystal-Clear-6-Pack/dp/B071Y48R19/ref=sr_1_11?keywords=60+watt+a19+incandescent+bulbs&amp;qid=1566159243&amp;s=gateway&amp;sr=8-11</t>
   </si>
   <si>
-    <t>C_op_base</t>
-  </si>
-  <si>
-    <t>C_op_EE</t>
-  </si>
-  <si>
-    <t>E_f</t>
-  </si>
-  <si>
-    <t>E_f_tot</t>
-  </si>
-  <si>
     <t>MJ/yr</t>
   </si>
   <si>
@@ -305,16 +563,43 @@
     <t>kW-hr/bulb</t>
   </si>
   <si>
-    <t>E_f_base</t>
-  </si>
-  <si>
-    <t>E_f_EE</t>
-  </si>
-  <si>
     <t>C_install</t>
   </si>
   <si>
     <t>Repl cost</t>
+  </si>
+  <si>
+    <t>C_repl_base</t>
+  </si>
+  <si>
+    <t>C_energy_base</t>
+  </si>
+  <si>
+    <t>C_energy_EE</t>
+  </si>
+  <si>
+    <t>C_repl_EE</t>
+  </si>
+  <si>
+    <t>E_f_energy_base</t>
+  </si>
+  <si>
+    <t>E_f_energy_EE</t>
+  </si>
+  <si>
+    <t>E_f_embodied_base</t>
+  </si>
+  <si>
+    <t>E_f_embodied_EE</t>
+  </si>
+  <si>
+    <t>E_f_emb_base</t>
+  </si>
+  <si>
+    <t>E_f_emb_EE</t>
+  </si>
+  <si>
+    <t>Heun</t>
   </si>
 </sst>
 </file>
@@ -338,12 +623,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color theme="1"/>
@@ -358,6 +637,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -391,8 +676,8 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
@@ -418,13 +703,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1029,15 +1314,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6945772-6A23-A140-A535-BB781130470A}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1048,22 +1343,37 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -1072,27 +1382,46 @@
         <v>3.0555555555555555E-2</v>
       </c>
       <c r="D2">
-        <f>Light!B22</f>
-        <v>10.08</v>
+        <f>Light!B15</f>
+        <v>7.23</v>
       </c>
       <c r="E2">
+        <f>Light!B20</f>
+        <v>2.85</v>
+      </c>
+      <c r="F2">
+        <f>Light!B43</f>
+        <v>1.02</v>
+      </c>
+      <c r="G2">
         <f>Light!B47</f>
-        <v>1.1032986111111112</v>
-      </c>
-      <c r="F2">
+        <v>8.3298611111111101E-2</v>
+      </c>
+      <c r="H2">
         <f>Light!B30</f>
-        <v>477.84199999999998</v>
-      </c>
-      <c r="G2">
+        <v>236.68200000000002</v>
+      </c>
+      <c r="I2">
+        <f>Light!B28</f>
+        <v>241.15999999999997</v>
+      </c>
+      <c r="J2">
+        <f>Light!B60</f>
+        <v>33.38181818181819</v>
+      </c>
+      <c r="K2">
         <f>Light!B58</f>
-        <v>69.555818181818196</v>
-      </c>
-      <c r="H2">
-        <f>Light!B60</f>
+        <v>36.173999999999999</v>
+      </c>
+      <c r="L2">
+        <f>Light!B64</f>
         <v>0.06</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -1105,10 +1434,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6332365-1DE6-2B42-AB77-F0F221D6C441}">
-  <dimension ref="A4:E82"/>
+  <dimension ref="A4:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1154,7 +1483,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3">
         <v>15.39</v>
@@ -1165,7 +1494,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <f>B10/6</f>
@@ -1250,7 +1579,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B20" s="6">
         <f>B11/B17</f>
@@ -1281,7 +1610,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="6"/>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1292,7 +1621,7 @@
         <v>60.29</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -1300,208 +1629,184 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B27">
         <f>B26/B17</f>
         <v>66.98888888888888</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B28">
+        <f>B27*MJ_per_kWhr</f>
+        <v>241.15999999999997</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29">
         <f>B13 / 1000 * B16 * 365.25</f>
         <v>65.745000000000005</v>
       </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29">
-        <f>B27+B28</f>
-        <v>132.73388888888888</v>
-      </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <f>B29*MJ_per_kWhr</f>
-        <v>477.84199999999998</v>
+        <v>236.68200000000002</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="3">
-        <v>23.99</v>
-      </c>
-      <c r="C35" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36">
-        <f>B35/24</f>
-        <v>0.99958333333333327</v>
-      </c>
-      <c r="C36" t="s">
-        <v>16</v>
-      </c>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B37" s="3">
-        <v>12</v>
+        <v>23.99</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B38" s="6">
-        <f>B37*B42*365.25</f>
-        <v>13090.909090909094</v>
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38">
+        <f>B37/24</f>
+        <v>0.99958333333333327</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B39" s="3">
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="6">
+        <f>B39*B44*365.25</f>
+        <v>13090.909090909094</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B41" s="3">
-        <v>1.02</v>
+        <v>8.5</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42">
-        <f>B41/B5 * 1000 / 365.25 / 8.5</f>
-        <v>2.9867463132350203</v>
-      </c>
-      <c r="C42" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B43" s="3">
-        <v>12</v>
+        <v>1.02</v>
       </c>
       <c r="C43" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B44" s="3"/>
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44">
+        <f>B43/B5 * 1000 / 365.25 / 8.5</f>
+        <v>2.9867463132350203</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45">
-        <f>B36/B43</f>
-        <v>8.3298611111111101E-2</v>
+        <v>22</v>
+      </c>
+      <c r="B45" s="3">
+        <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B46" s="3"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B47">
-        <f>B41+B45</f>
-        <v>1.1032986111111112</v>
+        <f>B38/B45</f>
+        <v>8.3298611111111101E-2</v>
       </c>
       <c r="C47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53" s="3">
-        <v>2</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54">
-        <f>B53*B26</f>
-        <v>120.58</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>48</v>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49">
+        <f>B43+B47</f>
+        <v>1.1032986111111112</v>
+      </c>
+      <c r="C49" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55">
-        <f>B54/B43</f>
-        <v>10.048333333333334</v>
-      </c>
-      <c r="C55" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="B55" s="3">
+        <v>2</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1509,50 +1814,74 @@
         <v>42</v>
       </c>
       <c r="B56">
-        <f>B39/1000 * B42 * 365.25</f>
-        <v>9.2727272727272751</v>
-      </c>
-      <c r="C56" t="s">
-        <v>38</v>
+        <f>B55*B26</f>
+        <v>120.58</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B57">
-        <f>B55+B56</f>
-        <v>19.321060606060609</v>
+        <f>B56/B45</f>
+        <v>10.048333333333334</v>
       </c>
       <c r="C57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B58">
         <f>B57*MJ_per_kWhr</f>
-        <v>69.555818181818196</v>
+        <v>36.173999999999999</v>
       </c>
       <c r="C58" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59">
+        <f>B41/1000 * B44 * 365.25</f>
+        <v>9.2727272727272751</v>
+      </c>
+      <c r="C59" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60">
+        <f>B59*MJ_per_kWhr</f>
+        <v>33.38181818181819</v>
+      </c>
+      <c r="C60" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>2</v>
       </c>
-      <c r="B60">
+      <c r="B64">
         <v>0.06</v>
       </c>
-      <c r="C60" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E82" t="s">
+      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E86" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>